<commit_message>
TR-50, TR-51 fix, doc
</commit_message>
<xml_diff>
--- a/docs/teszt/App tesztek.xlsx
+++ b/docs/teszt/App tesztek.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Különböző adatok megadása" sheetId="1" r:id="rId1"/>
-    <sheet name="Határérték teszt" sheetId="2" r:id="rId2"/>
+    <sheet name="TR-50 - TR-55 javítása" sheetId="3" r:id="rId2"/>
+    <sheet name="Határérték teszt" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="86">
   <si>
     <t>Funkcionális teszt</t>
   </si>
@@ -129,9 +130,6 @@
     <t>a = 13, b = 8, m = 6</t>
   </si>
   <si>
-    <t>a = 6 , e = 8, f = 7</t>
-  </si>
-  <si>
     <t>a = 6, b = 10, e = 8, f = 13</t>
   </si>
   <si>
@@ -204,9 +202,6 @@
     <t>K = 24, T = 35.8</t>
   </si>
   <si>
-    <t>K = 24, T = 28</t>
-  </si>
-  <si>
     <t>K = 32, T = 52</t>
   </si>
   <si>
@@ -256,6 +251,39 @@
   </si>
   <si>
     <t>K = 31, T = 44.04</t>
+  </si>
+  <si>
+    <t>a = 13, b = 7, c = 6, d = 7, m = 6.06</t>
+  </si>
+  <si>
+    <t>K = 33, T = 57.5</t>
+  </si>
+  <si>
+    <t>a = 5.32 , e = 8, f = 7</t>
+  </si>
+  <si>
+    <t>K = 21.2, T = 28</t>
+  </si>
+  <si>
+    <t>Rombsuz</t>
+  </si>
+  <si>
+    <t>TR-50</t>
+  </si>
+  <si>
+    <t>TR-51</t>
+  </si>
+  <si>
+    <t>TR-52</t>
+  </si>
+  <si>
+    <t>TR-53</t>
+  </si>
+  <si>
+    <t>TR-54</t>
+  </si>
+  <si>
+    <t>TR-55</t>
   </si>
 </sst>
 </file>
@@ -280,7 +308,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -357,11 +385,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,26 +443,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -709,14 +758,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -727,15 +776,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -774,10 +823,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>9</v>
@@ -816,10 +865,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>9</v>
@@ -829,7 +878,7 @@
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="18"/>
       <c r="D6" s="6" t="s">
         <v>14</v>
@@ -848,7 +897,7 @@
       <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -858,10 +907,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>9</v>
@@ -871,7 +920,7 @@
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
@@ -892,33 +941,33 @@
       <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="6" t="s">
         <v>30</v>
       </c>
@@ -939,7 +988,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -949,10 +998,10 @@
         <v>32</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>9</v>
@@ -962,7 +1011,7 @@
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="6" t="s">
         <v>30</v>
       </c>
@@ -983,7 +1032,7 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -993,10 +1042,10 @@
         <v>33</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>9</v>
@@ -1006,7 +1055,7 @@
       <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1027,33 +1076,30 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6" t="s">
         <v>30</v>
       </c>
@@ -1064,31 +1110,33 @@
         <v>15</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="22"/>
+        <v>52</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>9</v>
@@ -1098,7 +1146,7 @@
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1109,33 +1157,33 @@
         <v>15</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>9</v>
@@ -1145,7 +1193,7 @@
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="6" t="s">
         <v>30</v>
       </c>
@@ -1166,33 +1214,33 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="6" t="s">
         <v>30</v>
       </c>
@@ -1213,33 +1261,33 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="6" t="s">
         <v>30</v>
       </c>
@@ -1260,33 +1308,33 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="22" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="6" t="s">
         <v>30</v>
       </c>
@@ -1304,13 +1352,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
+  <mergeCells count="13">
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
@@ -1319,12 +1361,145 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -1341,111 +1516,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="A1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>47</v>
+      <c r="A3" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="B3" s="13">
         <v>-1</v>
       </c>
       <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="13">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="13">
         <v>1073741823</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="13">
         <v>2147483647</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="13">
         <v>2147483648</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>

</xml_diff>

<commit_message>
TR-52 - TR-55 fix, docs
</commit_message>
<xml_diff>
--- a/docs/teszt/App tesztek.xlsx
+++ b/docs/teszt/App tesztek.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="91">
   <si>
     <t>Funkcionális teszt</t>
   </si>
@@ -284,6 +284,21 @@
   </si>
   <si>
     <t>TR-55</t>
+  </si>
+  <si>
+    <t>m = 20, r = 5</t>
+  </si>
+  <si>
+    <t>m = 20, a = 5</t>
+  </si>
+  <si>
+    <t>A = 1884.96, V = 6283.19</t>
+  </si>
+  <si>
+    <t>A = 42.32, V = 165</t>
+  </si>
+  <si>
+    <t>A = 1256.6, V = 3141.59</t>
   </si>
 </sst>
 </file>
@@ -398,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,6 +462,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -455,26 +488,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,7 +780,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,15 +797,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -813,7 +834,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -836,7 +857,7 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -857,8 +878,8 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="23" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -878,8 +899,8 @@
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
@@ -897,7 +918,7 @@
       <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -920,7 +941,7 @@
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
@@ -941,7 +962,7 @@
       <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -967,7 +988,7 @@
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="6" t="s">
         <v>30</v>
       </c>
@@ -988,7 +1009,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -1011,7 +1032,7 @@
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="20"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1032,7 +1053,7 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -1055,7 +1076,7 @@
       <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1076,7 +1097,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1092,14 +1113,14 @@
         <v>78</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="20"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="6" t="s">
         <v>30</v>
       </c>
@@ -1115,7 +1136,7 @@
       <c r="G16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="18" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1123,7 +1144,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1146,7 +1167,7 @@
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1170,7 +1191,7 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -1193,7 +1214,7 @@
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="6" t="s">
         <v>30</v>
       </c>
@@ -1214,7 +1235,7 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -1230,7 +1251,7 @@
         <v>59</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>67</v>
@@ -1240,7 +1261,7 @@
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="6" t="s">
         <v>30</v>
       </c>
@@ -1261,7 +1282,7 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -1277,7 +1298,7 @@
         <v>62</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>63</v>
@@ -1287,7 +1308,7 @@
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="20"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="6" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1329,7 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -1324,7 +1345,7 @@
         <v>70</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>69</v>
@@ -1334,7 +1355,7 @@
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="20"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="6" t="s">
         <v>30</v>
       </c>
@@ -1353,6 +1374,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
@@ -1361,11 +1387,6 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1376,30 +1397,29 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="19" customWidth="1"/>
     <col min="3" max="3" width="52.85546875" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1443,7 +1463,7 @@
       <c r="F3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="20" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1474,20 +1494,92 @@
       <c r="A5" s="16" t="s">
         <v>82</v>
       </c>
+      <c r="B5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>83</v>
       </c>
+      <c r="B6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>84</v>
       </c>
+      <c r="B7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>85</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1516,13 +1608,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1542,7 +1634,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="13">
@@ -1559,7 +1651,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="13">
         <v>0</v>
       </c>
@@ -1574,7 +1666,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="13">
         <v>1073741823</v>
       </c>
@@ -1589,7 +1681,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="13">
         <v>2147483647</v>
       </c>
@@ -1604,7 +1696,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="13">
         <v>2147483648</v>
       </c>

</xml_diff>